<commit_message>
informe fin de dia
</commit_message>
<xml_diff>
--- a/descargas/informe.xlsx
+++ b/descargas/informe.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="B1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,84 +436,48 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Fecha</t>
+          <t>Chofer</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Seguimiento</t>
+          <t>En_camino_hoy</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>comprador</t>
+          <t>Entregados</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Direccion</t>
+          <t>Nadie_en_domicilio</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Localidad</t>
+          <t>No_visitado</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Estado</t>
+          <t>Diferencia_cargados_Entregados</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Motivo</t>
+          <t>Horario_salida</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Monto</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>44932</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NOML13315050838</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CLIENTE DE AVELLANEDA</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Comodoro Rivadavia 2385</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Avellaneda</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Entregado</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Entregado sin novedades</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>8000</v>
+          <t>Horario_fin</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>efectividad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>